<commit_message>
added colors to diagnosis
</commit_message>
<xml_diff>
--- a/resources/ca.xlsx
+++ b/resources/ca.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perema\Documents\Projects\legacy_webapp\TRICC-Webapp\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\perema\Documents\Projects\MSFeCARE\forms-clinical\ped\release_ped_v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="62">
   <si>
     <t>cond1</t>
   </si>
@@ -209,7 +209,7 @@
     <t>d_vomit_no_dehydration</t>
   </si>
   <si>
-    <t>d_cystitis_acute</t>
+    <t>d_lower_uti</t>
   </si>
 </sst>
 </file>
@@ -542,8 +542,8 @@
   <dimension ref="A1:AMJ48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -817,9 +817,6 @@
       <c r="A20" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="1" t="s">
-        <v>15</v>
-      </c>
       <c r="M20" s="1" t="s">
         <v>15</v>
       </c>
@@ -843,9 +840,6 @@
     <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="M23" s="1" t="s">
         <v>15</v>

</xml_diff>